<commit_message>
add mandatory person affiliation (closes #17 )
</commit_message>
<xml_diff>
--- a/tests/fixtures/test-arc/isa.investigation.xlsx
+++ b/tests/fixtures/test-arc/isa.investigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schne\source\repos\nfdi4plants\arc-to-invenio\tests\fixtures\test-arc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE16671-7DCB-4D70-8F00-3563A5E75BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B199593-371D-4DBE-8E76-164BC8B86364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43380" yWindow="3330" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="110">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -344,13 +344,19 @@
   </si>
   <si>
     <t>0000-0000-0000-0000</t>
+  </si>
+  <si>
+    <t>Institute 1</t>
+  </si>
+  <si>
+    <t>Institute 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,6 +487,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -783,7 +797,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -826,11 +840,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -864,6 +880,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1186,14 +1203,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1348,7 +1366,7 @@
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C24" t="s">
@@ -1393,10 +1411,10 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1759,7 +1777,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B24" r:id="rId1" xr:uid="{5EE387A2-DC41-4C1C-9EA1-C5FC25FA4A4F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add mandatory description field
</commit_message>
<xml_diff>
--- a/tests/fixtures/test-arc/isa.investigation.xlsx
+++ b/tests/fixtures/test-arc/isa.investigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schne\source\repos\nfdi4plants\arc-to-invenio\tests\fixtures\test-arc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B199593-371D-4DBE-8E76-164BC8B86364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B55D2E-36AC-4639-A505-14ED0E75F57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43380" yWindow="3330" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -1204,7 +1204,7 @@
   <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>